<commit_message>
alpha, beta, and sharpe ratio
</commit_message>
<xml_diff>
--- a/app/ETFTrader/comparison.xlsx
+++ b/app/ETFTrader/comparison.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26819"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14340" tabRatio="500"/>
+    <workbookView xWindow="5280" yWindow="0" windowWidth="14680" windowHeight="14340" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Account" sheetId="1" r:id="rId1"/>
+    <sheet name="EOM" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="23">
   <si>
     <t>Date</t>
   </si>
@@ -71,12 +72,30 @@
   <si>
     <t>Buy XLY</t>
   </si>
+  <si>
+    <t>Copy from code output</t>
+  </si>
+  <si>
+    <t>Manual calculation</t>
+  </si>
+  <si>
+    <t>Portfolio($)</t>
+  </si>
+  <si>
+    <t>Portfolio(%)</t>
+  </si>
+  <si>
+    <t>Equity(%)</t>
+  </si>
+  <si>
+    <t>Rf(%)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -100,6 +119,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -118,7 +151,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="19">
+  <cellStyleXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -138,13 +171,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="19">
+  <cellStyles count="23">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -154,6 +193,8 @@
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -163,6 +204,8 @@
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -494,7 +537,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X162"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="K70" activeCellId="7" sqref="A14 K14 A35 K35 A56 K56 A70 K70"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
@@ -1044,6 +1089,12 @@
       <c r="D12" t="s">
         <v>6</v>
       </c>
+      <c r="H12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="N12" s="3" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="13" spans="1:24">
       <c r="A13" t="s">
@@ -1224,14 +1275,14 @@
         <v>923.33000200000015</v>
       </c>
       <c r="I16" s="2">
-        <f t="shared" ref="I16:I75" si="12">F16</f>
+        <f t="shared" ref="I16:I56" si="12">F16</f>
         <v>76.489998</v>
       </c>
       <c r="J16" s="2">
         <v>0</v>
       </c>
       <c r="K16" s="2">
-        <f t="shared" ref="K16:K75" si="13">SUM(H16:J16)</f>
+        <f t="shared" ref="K16:K70" si="13">SUM(H16:J16)</f>
         <v>999.82000000000016</v>
       </c>
       <c r="N16">
@@ -4155,6 +4206,126 @@
     <row r="162" spans="1:4">
       <c r="A162" s="1"/>
       <c r="D162" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="1">
+        <v>42216</v>
+      </c>
+      <c r="B2">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="1">
+        <v>42247</v>
+      </c>
+      <c r="B3" s="2">
+        <v>993.82000000000016</v>
+      </c>
+      <c r="C3">
+        <f>(B3-B2)/B2*100</f>
+        <v>-0.61799999999998367</v>
+      </c>
+      <c r="D3">
+        <v>-6.2580818167202406</v>
+      </c>
+      <c r="F3">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="1">
+        <v>42277</v>
+      </c>
+      <c r="B4" s="2">
+        <v>989.56000500000016</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:C5" si="0">(B4-B3)/B3*100</f>
+        <v>-0.42864854802680591</v>
+      </c>
+      <c r="D4">
+        <v>-2.6442831573227021</v>
+      </c>
+      <c r="F4">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1">
+        <v>42297</v>
+      </c>
+      <c r="B5" s="2">
+        <v>993.97999600000003</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>0.44666225167415369</v>
+      </c>
+      <c r="D5">
+        <v>5.7676176584423589</v>
+      </c>
+      <c r="F5" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="C7">
+        <f>1+C3/100</f>
+        <v>0.99382000000000015</v>
+      </c>
+      <c r="D7">
+        <f>1+D3/100</f>
+        <v>0.9374191818327976</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="C8">
+        <f>C7^12</f>
+        <v>0.92830948696108184</v>
+      </c>
+      <c r="D8">
+        <f>D7^12</f>
+        <v>0.46047497365828416</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>